<commit_message>
add further relation values for RWGS and FT
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/01_input_raw/diesel/Model_Data_Base_diesel_4_InOutputs.xlsx
+++ b/Spine_Projects/01_input_data/01_input_raw/diesel/Model_Data_Base_diesel_4_InOutputs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentcbs-my.sharepoint.com/personal/luc_eco_cbs_dk/Documents/Documents/GitHub/Nord_H2ub/Spine_Projects/01_input_data/01_input_raw/diesel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfg.eco\Documents\GitHub\Nord_H2ub\spine_projects\01_input_data\01_input_raw\diesel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="129" documentId="13_ncr:1_{B63BCB0A-9012-4F55-92B6-F45564B797E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{67EE8BD9-BD2F-4902-9840-26D629B2CBAC}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E38B92B-F50E-4E68-9BEB-7AC5EC652D2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-1560" yWindow="-19440" windowWidth="38700" windowHeight="15315" activeTab="3" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
+    <workbookView xWindow="-5070" yWindow="-21720" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
   </bookViews>
   <sheets>
     <sheet name="Units" sheetId="1" r:id="rId1"/>
@@ -54,6 +54,7 @@
     <definedName name="IQ_YTDMONTH" hidden="1">130000</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -74,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="125">
   <si>
     <t>Unit</t>
   </si>
@@ -343,15 +344,9 @@
     <t>heat_high</t>
   </si>
   <si>
-    <t>heat_split</t>
-  </si>
-  <si>
     <t>Auxilliary</t>
   </si>
   <si>
-    <t>internal_heat</t>
-  </si>
-  <si>
     <t>Input3</t>
   </si>
   <si>
@@ -452,6 +447,9 @@
   </si>
   <si>
     <t>diesel_st</t>
+  </si>
+  <si>
+    <t>co2_source</t>
   </si>
 </sst>
 </file>
@@ -1701,7 +1699,7 @@
   <dimension ref="A1:R12"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1727,7 +1725,7 @@
         <v>43</v>
       </c>
       <c r="C1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D1" t="s">
         <v>12</v>
@@ -1736,16 +1734,16 @@
         <v>13</v>
       </c>
       <c r="F1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="G1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="H1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="I1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="J1" t="s">
         <v>64</v>
@@ -1790,7 +1788,7 @@
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B3" t="s">
         <v>62</v>
@@ -1803,7 +1801,7 @@
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B4" t="s">
         <v>63</v>
@@ -1844,7 +1842,7 @@
         <v>25</v>
       </c>
       <c r="C6" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="P6" s="1"/>
       <c r="Q6" s="1"/>
@@ -1857,7 +1855,7 @@
         <v>68</v>
       </c>
       <c r="C7" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="P7" s="1" t="s">
         <v>42</v>
@@ -1868,10 +1866,10 @@
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B8" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C8" t="s">
         <v>78</v>
@@ -1897,10 +1895,10 @@
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C10" t="s">
         <v>75</v>
@@ -1913,10 +1911,10 @@
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B11" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C11" t="s">
         <v>82</v>
@@ -1929,13 +1927,13 @@
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B12" t="s">
-        <v>113</v>
-      </c>
-      <c r="C12" t="s">
-        <v>121</v>
+        <v>111</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>117</v>
       </c>
       <c r="P12" s="1"/>
       <c r="Q12" s="1"/>
@@ -1969,10 +1967,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CABA7C5-6230-4207-9D35-0A95D86E66AC}">
-  <dimension ref="A1:Q13"/>
+  <dimension ref="A1:Q12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1996,10 +1994,10 @@
         <v>2</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="G1" s="5" t="s">
         <v>3</v>
@@ -2008,31 +2006,31 @@
         <v>4</v>
       </c>
       <c r="I1" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="K1" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="L1" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="M1" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="N1" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="O1" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="P1" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="Q1" s="5" t="s">
         <v>100</v>
-      </c>
-      <c r="P1" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="Q1" s="5" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.35">
@@ -2062,7 +2060,7 @@
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>62</v>
@@ -2087,7 +2085,7 @@
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B4" t="s">
         <v>63</v>
@@ -2186,21 +2184,27 @@
         <v>68</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D7" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="E7" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="E7" s="4"/>
       <c r="F7" s="4"/>
       <c r="G7" s="4" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
+        <v>121</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>87</v>
+      </c>
       <c r="K7" s="4"/>
       <c r="L7" s="4"/>
       <c r="M7" s="4"/>
@@ -2211,10 +2215,10 @@
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B8" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>78</v>
@@ -2222,13 +2226,19 @@
       <c r="D8" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="E8" s="3"/>
+      <c r="E8" s="3" t="s">
+        <v>70</v>
+      </c>
       <c r="F8" s="3"/>
       <c r="G8" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
+        <v>119</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>88</v>
+      </c>
       <c r="J8" s="3"/>
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
@@ -2273,27 +2283,33 @@
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B10" t="s">
-        <v>90</v>
+        <v>89</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B11" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>111</v>
+        <v>124</v>
       </c>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
       <c r="G11" s="4" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
@@ -2310,27 +2326,35 @@
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B12" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="D12" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
+      <c r="D12" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>76</v>
+      </c>
       <c r="G12" s="6" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="H12" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="I12" s="6"/>
-      <c r="J12" s="6"/>
+      <c r="I12" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>75</v>
+      </c>
       <c r="K12" s="6"/>
       <c r="L12" s="6"/>
       <c r="M12" s="6"/>
@@ -2338,37 +2362,6 @@
       <c r="O12" s="6"/>
       <c r="P12" s="6"/>
       <c r="Q12" s="6"/>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A13" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="H13" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="I13" s="6"/>
-      <c r="J13" s="6"/>
-      <c r="K13" s="6"/>
-      <c r="L13" s="6"/>
-      <c r="M13" s="6"/>
-      <c r="N13" s="6"/>
-      <c r="O13" s="6">
-        <v>1</v>
-      </c>
-      <c r="P13" s="6"/>
-      <c r="Q13" s="6"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -2383,7 +2376,7 @@
           <x14:formula1>
             <xm:f>Drop_Down!$A:$A</xm:f>
           </x14:formula1>
-          <xm:sqref>B13 B1:B12</xm:sqref>
+          <xm:sqref>B1:B12</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2625,22 +2618,22 @@
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C4" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F4" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="G4" t="s">
         <v>32</v>
@@ -2710,7 +2703,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{981CFA5E-60F3-446F-A856-2FA65B76879A}">
   <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
@@ -2792,10 +2785,10 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -2941,32 +2934,32 @@
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adjust relation values for FT products
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/01_input_raw/diesel/Model_Data_Base_diesel_4_InOutputs.xlsx
+++ b/Spine_Projects/01_input_data/01_input_raw/diesel/Model_Data_Base_diesel_4_InOutputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfg.eco\Documents\GitHub\Nord_H2ub\spine_projects\01_input_data\01_input_raw\diesel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EFBB702-96F4-4C4C-9123-6AF6ADCEE697}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D337359F-EBFB-4147-8D93-3C3B73BAD1B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
   </bookViews>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="125">
   <si>
     <t>Unit</t>
   </si>
@@ -1969,7 +1969,7 @@
   <dimension ref="A1:Q12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="P15" sqref="P15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2188,9 +2188,7 @@
       <c r="D7" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="E7" s="4" t="s">
-        <v>88</v>
-      </c>
+      <c r="E7" s="4"/>
       <c r="F7" s="4"/>
       <c r="G7" s="4" t="s">
         <v>120</v>
@@ -2198,12 +2196,8 @@
       <c r="H7" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="I7" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="J7" s="4" t="s">
-        <v>87</v>
-      </c>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
       <c r="K7" s="4"/>
       <c r="L7" s="4"/>
       <c r="M7" s="4"/>
@@ -2228,16 +2222,14 @@
       <c r="E8" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="F8" s="3"/>
+      <c r="F8" s="3" t="s">
+        <v>76</v>
+      </c>
       <c r="G8" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="H8" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="I8" s="3" t="s">
-        <v>88</v>
-      </c>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
       <c r="J8" s="3"/>
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
@@ -2344,13 +2336,13 @@
         <v>117</v>
       </c>
       <c r="H12" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="I12" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="I12" s="4" t="s">
+      <c r="J12" s="3" t="s">
         <v>87</v>
-      </c>
-      <c r="J12" s="3" t="s">
-        <v>75</v>
       </c>
       <c r="K12" s="6"/>
       <c r="L12" s="6"/>

</xml_diff>

<commit_message>
add relation values to input for diesel
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/01_input_raw/diesel/Model_Data_Base_diesel_4_InOutputs.xlsx
+++ b/Spine_Projects/01_input_data/01_input_raw/diesel/Model_Data_Base_diesel_4_InOutputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfg.eco\Documents\GitHub\Nord_H2ub\spine_projects\01_input_data\01_input_raw\diesel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D337359F-EBFB-4147-8D93-3C3B73BAD1B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03E8FAFA-5122-4C31-B5F7-0204A3774FC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
   </bookViews>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="127">
   <si>
     <t>Unit</t>
   </si>
@@ -449,6 +449,12 @@
   </si>
   <si>
     <t>co2_source</t>
+  </si>
+  <si>
+    <t>heat_recovery</t>
+  </si>
+  <si>
+    <t>power_steam</t>
   </si>
 </sst>
 </file>
@@ -539,7 +545,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -552,6 +558,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1305,8 +1312,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{C1664CC4-80CB-414D-BAFE-57FF9635D79F}" name="Table5" displayName="Table5" ref="A1:Q12" totalsRowShown="0" headerRowDxfId="24" dataDxfId="22" headerRowBorderDxfId="23" tableBorderDxfId="21" totalsRowBorderDxfId="20">
-  <autoFilter ref="A1:Q12" xr:uid="{C1664CC4-80CB-414D-BAFE-57FF9635D79F}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{C1664CC4-80CB-414D-BAFE-57FF9635D79F}" name="Table5" displayName="Table5" ref="A1:Q14" totalsRowShown="0" headerRowDxfId="24" dataDxfId="22" headerRowBorderDxfId="23" tableBorderDxfId="21" totalsRowBorderDxfId="20">
+  <autoFilter ref="A1:Q14" xr:uid="{C1664CC4-80CB-414D-BAFE-57FF9635D79F}"/>
   <tableColumns count="17">
     <tableColumn id="1" xr3:uid="{2BE3E317-773B-4E82-9035-69A43C6CB21B}" name="Unit" dataDxfId="19"/>
     <tableColumn id="2" xr3:uid="{22613EE0-390D-4B04-9A9B-6D5554D1C8ED}" name="Object_type" dataDxfId="18"/>
@@ -1966,10 +1973,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CABA7C5-6230-4207-9D35-0A95D86E66AC}">
-  <dimension ref="A1:Q12"/>
+  <dimension ref="A1:Q14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P15" sqref="P15"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2198,11 +2205,17 @@
       </c>
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
-      <c r="K7" s="4"/>
+      <c r="K7" s="4">
+        <v>161.1904761904762</v>
+      </c>
       <c r="L7" s="4"/>
       <c r="M7" s="4"/>
-      <c r="N7" s="4"/>
-      <c r="O7" s="4"/>
+      <c r="N7" s="4">
+        <v>1.6666666666666667</v>
+      </c>
+      <c r="O7" s="4">
+        <v>1.4999999999999998</v>
+      </c>
       <c r="P7" s="4"/>
       <c r="Q7" s="4"/>
     </row>
@@ -2231,10 +2244,18 @@
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3"/>
-      <c r="M8" s="3"/>
-      <c r="N8" s="3"/>
+      <c r="K8" s="3">
+        <v>2.8982576753129519</v>
+      </c>
+      <c r="L8" s="3">
+        <v>12.285714285714285</v>
+      </c>
+      <c r="M8" s="3">
+        <v>3.0714285714285712</v>
+      </c>
+      <c r="N8" s="3">
+        <v>0.86</v>
+      </c>
       <c r="O8" s="3"/>
       <c r="P8" s="3"/>
       <c r="Q8" s="3"/>
@@ -2247,7 +2268,7 @@
         <v>45</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>70</v>
+        <v>126</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>75</v>
@@ -2261,12 +2282,12 @@
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
       <c r="K9" s="4">
-        <v>7.2437800000000002E-4</v>
+        <v>9.8530247749999979E-4</v>
       </c>
       <c r="L9" s="4"/>
       <c r="M9" s="4"/>
       <c r="N9" s="4">
-        <v>0.99</v>
+        <v>1.0101010101010102</v>
       </c>
       <c r="O9" s="4"/>
       <c r="P9" s="4"/>
@@ -2284,6 +2305,9 @@
       </c>
       <c r="G10" s="4" t="s">
         <v>75</v>
+      </c>
+      <c r="N10">
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.35">
@@ -2344,13 +2368,81 @@
       <c r="J12" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="K12" s="6"/>
-      <c r="L12" s="6"/>
+      <c r="K12" s="6">
+        <v>42.75</v>
+      </c>
+      <c r="L12" s="6">
+        <v>1.6132075471698113</v>
+      </c>
       <c r="M12" s="6"/>
-      <c r="N12" s="6"/>
-      <c r="O12" s="6"/>
-      <c r="P12" s="6"/>
+      <c r="N12" s="6">
+        <v>1.6285714285714283</v>
+      </c>
+      <c r="O12" s="6">
+        <v>6.7340067340067344</v>
+      </c>
+      <c r="P12" s="6">
+        <v>5.5096418732782366</v>
+      </c>
       <c r="Q12" s="6"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A13" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="4"/>
+      <c r="K13" s="4"/>
+      <c r="L13" s="4"/>
+      <c r="M13" s="4"/>
+      <c r="N13" s="4">
+        <v>1.1883541295306002</v>
+      </c>
+      <c r="O13" s="4"/>
+      <c r="P13" s="4"/>
+      <c r="Q13" s="4"/>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A14" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="8"/>
+      <c r="L14" s="8"/>
+      <c r="M14" s="8"/>
+      <c r="N14" s="8">
+        <v>1</v>
+      </c>
+      <c r="O14" s="8"/>
+      <c r="P14" s="8"/>
+      <c r="Q14" s="8"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -2365,7 +2457,7 @@
           <x14:formula1>
             <xm:f>Drop_Down!$A:$A</xm:f>
           </x14:formula1>
-          <xm:sqref>B1:B12</xm:sqref>
+          <xm:sqref>B1:B14</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>